<commit_message>
added Images folder with test image
</commit_message>
<xml_diff>
--- a/Data/data-entry-final.xlsx
+++ b/Data/data-entry-final.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3edad19b159922f5/_Documents/2021W/Bamfield/MPED/Coding/Git_Repos/biodiv-sampling-intertidal_height/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3edad19b159922f5/_Documents/2021W/Bamfield/MPED/Coding/Git_Repos/biodiversity-sampling-intertidal-height/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="10" documentId="8_{0BBD40F6-9FEB-CB48-AE75-A5C679CCEBCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B917F580-E4BF-CA49-9A6A-D83A39659012}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="quadrat-data" sheetId="1" r:id="rId1"/>

</xml_diff>